<commit_message>
added menu selection prototype. need to add buttons and design overall layout tomorrow
</commit_message>
<xml_diff>
--- a/data/teamhistory.xlsx
+++ b/data/teamhistory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="222">
   <si>
     <t>TEAM_ID</t>
   </si>
@@ -679,6 +679,12 @@
   </si>
   <si>
     <t>#C2CCCC</t>
+  </si>
+  <si>
+    <t>TOR</t>
+  </si>
+  <si>
+    <t>GOS</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U75"/>
+  <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2375,7 +2381,7 @@
         <v>2</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2386,46 +2392,46 @@
         <v>1610612744</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="3">
-        <v>1962</v>
+        <v>1971</v>
       </c>
       <c r="F24" s="3">
-        <v>1970</v>
+        <v>2016</v>
       </c>
       <c r="G24" s="3">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="H24" s="3">
-        <v>729</v>
+        <v>3649</v>
       </c>
       <c r="I24" s="3">
-        <v>330</v>
+        <v>1707</v>
       </c>
       <c r="J24" s="3">
-        <v>399</v>
+        <v>1942</v>
       </c>
       <c r="K24" s="3">
-        <v>0.45200000000000001</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="L24" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="M24" s="3">
+        <v>4</v>
+      </c>
+      <c r="N24" s="3">
+        <v>3</v>
+      </c>
+      <c r="O24" s="3">
         <v>2</v>
       </c>
-      <c r="N24" s="3">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3">
-        <v>0</v>
-      </c>
       <c r="P24" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2436,161 +2442,161 @@
         <v>1610612744</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E25" s="3">
+        <v>1962</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1970</v>
+      </c>
+      <c r="G25" s="3">
+        <v>9</v>
+      </c>
+      <c r="H25" s="3">
+        <v>729</v>
+      </c>
+      <c r="I25" s="3">
+        <v>330</v>
+      </c>
+      <c r="J25" s="3">
+        <v>399</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="L25" s="3">
+        <v>5</v>
+      </c>
+      <c r="M25" s="3">
+        <v>2</v>
+      </c>
+      <c r="N25" s="3">
+        <v>0</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0</v>
+      </c>
+      <c r="P25" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1610612744</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="3">
         <v>1946</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F26" s="3">
         <v>1961</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G26" s="3">
         <v>16</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H26" s="3">
         <v>1103</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I26" s="3">
         <v>558</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J26" s="3">
         <v>545</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K26" s="3">
         <v>0.505</v>
       </c>
-      <c r="L25" s="3">
+      <c r="L26" s="3">
         <v>12</v>
       </c>
-      <c r="M25" s="3">
+      <c r="M26" s="3">
         <v>3</v>
       </c>
-      <c r="N25" s="3">
-        <v>0</v>
-      </c>
-      <c r="O25" s="3">
+      <c r="N26" s="3">
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
         <v>2</v>
       </c>
-      <c r="P25" s="6" t="s">
+      <c r="P26" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:21">
+      <c r="A27" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B27" s="4">
         <v>1610612745</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E27" s="4">
         <v>1967</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F27" s="4">
         <v>2016</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G27" s="4">
         <v>50</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H27" s="4">
         <v>3977</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I27" s="4">
         <v>2056</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J27" s="4">
         <v>1921</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K27" s="4">
         <v>0.51600000000000001</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L27" s="4">
         <v>30</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M27" s="4">
         <v>5</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N27" s="4">
         <v>4</v>
       </c>
-      <c r="O26" s="4">
+      <c r="O27" s="4">
         <v>2</v>
       </c>
-      <c r="P26" s="4" t="s">
+      <c r="P27" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="R27" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="S26" s="3" t="s">
+      <c r="S27" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="T26" s="3" t="s">
+      <c r="T27" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="U26" s="3" t="s">
+      <c r="U27" s="3" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B27" s="3">
-        <v>1610612745</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1971</v>
-      </c>
-      <c r="F27" s="3">
-        <v>2016</v>
-      </c>
-      <c r="G27" s="3">
-        <v>46</v>
-      </c>
-      <c r="H27" s="3">
-        <v>3649</v>
-      </c>
-      <c r="I27" s="3">
-        <v>1937</v>
-      </c>
-      <c r="J27" s="3">
-        <v>1712</v>
-      </c>
-      <c r="K27" s="3">
-        <v>0.53</v>
-      </c>
-      <c r="L27" s="3">
-        <v>29</v>
-      </c>
-      <c r="M27" s="3">
-        <v>5</v>
-      </c>
-      <c r="N27" s="3">
-        <v>4</v>
-      </c>
-      <c r="O27" s="3">
-        <v>2</v>
-      </c>
-      <c r="P27" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -2601,108 +2607,96 @@
         <v>1610612745</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="3">
+        <v>1971</v>
+      </c>
+      <c r="F28" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G28" s="3">
+        <v>46</v>
+      </c>
+      <c r="H28" s="3">
+        <v>3649</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1937</v>
+      </c>
+      <c r="J28" s="3">
+        <v>1712</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.53</v>
+      </c>
+      <c r="L28" s="3">
+        <v>29</v>
+      </c>
+      <c r="M28" s="3">
+        <v>5</v>
+      </c>
+      <c r="N28" s="3">
+        <v>4</v>
+      </c>
+      <c r="O28" s="3">
+        <v>2</v>
+      </c>
+      <c r="P28" s="6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1610612745</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E29" s="3">
         <v>1967</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F29" s="3">
         <v>1970</v>
       </c>
-      <c r="G28" s="3">
+      <c r="G29" s="3">
         <v>4</v>
       </c>
-      <c r="H28" s="3">
+      <c r="H29" s="3">
         <v>328</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I29" s="3">
         <v>119</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J29" s="3">
         <v>209</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K29" s="3">
         <v>0.36199999999999999</v>
       </c>
-      <c r="L28" s="3">
+      <c r="L29" s="3">
         <v>1</v>
       </c>
-      <c r="M28" s="3">
-        <v>0</v>
-      </c>
-      <c r="N28" s="3">
-        <v>0</v>
-      </c>
-      <c r="O28" s="3">
-        <v>0</v>
-      </c>
-      <c r="P28" s="6" t="s">
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0</v>
+      </c>
+      <c r="P29" s="6" t="s">
         <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B29" s="4">
-        <v>1610612754</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E29" s="4">
-        <v>1976</v>
-      </c>
-      <c r="F29" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G29" s="4">
-        <v>41</v>
-      </c>
-      <c r="H29" s="4">
-        <v>3239</v>
-      </c>
-      <c r="I29" s="4">
-        <v>1609</v>
-      </c>
-      <c r="J29" s="4">
-        <v>1629</v>
-      </c>
-      <c r="K29" s="4">
-        <v>0.496</v>
-      </c>
-      <c r="L29" s="4">
-        <v>23</v>
-      </c>
-      <c r="M29" s="4">
-        <v>6</v>
-      </c>
-      <c r="N29" s="4">
-        <v>1</v>
-      </c>
-      <c r="O29" s="4">
-        <v>0</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="R29" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="S29" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="T29" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -2710,55 +2704,55 @@
         <v>177</v>
       </c>
       <c r="B30" s="4">
-        <v>1610612746</v>
+        <v>1610612754</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E30" s="4">
-        <v>1970</v>
+        <v>1976</v>
       </c>
       <c r="F30" s="4">
         <v>2016</v>
       </c>
       <c r="G30" s="4">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H30" s="4">
-        <v>3731</v>
+        <v>3239</v>
       </c>
       <c r="I30" s="4">
-        <v>1475</v>
+        <v>1609</v>
       </c>
       <c r="J30" s="4">
-        <v>2256</v>
+        <v>1629</v>
       </c>
       <c r="K30" s="4">
-        <v>0.39500000000000002</v>
+        <v>0.496</v>
       </c>
       <c r="L30" s="4">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="M30" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N30" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="4">
         <v>0</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="R30" s="3" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="S30" s="3" t="s">
         <v>191</v>
@@ -2766,58 +2760,70 @@
       <c r="T30" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="U30" s="3" t="s">
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1610612746</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1970</v>
+      </c>
+      <c r="F31" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G31" s="4">
+        <v>47</v>
+      </c>
+      <c r="H31" s="4">
+        <v>3731</v>
+      </c>
+      <c r="I31" s="4">
+        <v>1475</v>
+      </c>
+      <c r="J31" s="4">
+        <v>2256</v>
+      </c>
+      <c r="K31" s="4">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="L31" s="4">
+        <v>12</v>
+      </c>
+      <c r="M31" s="4">
+        <v>3</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" s="4">
+        <v>0</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="S31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="T31" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="U31" s="3" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1610612746</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="3">
-        <v>2015</v>
-      </c>
-      <c r="F31" s="3">
-        <v>2016</v>
-      </c>
-      <c r="G31" s="3">
-        <v>2</v>
-      </c>
-      <c r="H31" s="3">
-        <v>89</v>
-      </c>
-      <c r="I31" s="3">
-        <v>59</v>
-      </c>
-      <c r="J31" s="3">
-        <v>30</v>
-      </c>
-      <c r="K31" s="3">
-        <v>0.66200000000000003</v>
-      </c>
-      <c r="L31" s="3">
-        <v>1</v>
-      </c>
-      <c r="M31" s="3">
-        <v>1</v>
-      </c>
-      <c r="N31" s="3">
-        <v>0</v>
-      </c>
-      <c r="O31" s="3">
-        <v>0</v>
-      </c>
-      <c r="P31" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -2834,31 +2840,31 @@
         <v>49</v>
       </c>
       <c r="E32" s="3">
-        <v>1984</v>
+        <v>2015</v>
       </c>
       <c r="F32" s="3">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="G32" s="3">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="H32" s="3">
-        <v>2494</v>
+        <v>89</v>
       </c>
       <c r="I32" s="3">
-        <v>971</v>
+        <v>59</v>
       </c>
       <c r="J32" s="3">
-        <v>1523</v>
+        <v>30</v>
       </c>
       <c r="K32" s="3">
-        <v>0.38900000000000001</v>
+        <v>0.66200000000000003</v>
       </c>
       <c r="L32" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M32" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N32" s="3">
         <v>0</v>
@@ -2878,37 +2884,37 @@
         <v>1610612746</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E33" s="3">
-        <v>1978</v>
+        <v>1984</v>
       </c>
       <c r="F33" s="3">
-        <v>1983</v>
+        <v>2014</v>
       </c>
       <c r="G33" s="3">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="H33" s="3">
-        <v>492</v>
+        <v>2494</v>
       </c>
       <c r="I33" s="3">
-        <v>186</v>
+        <v>971</v>
       </c>
       <c r="J33" s="3">
-        <v>306</v>
+        <v>1523</v>
       </c>
       <c r="K33" s="3">
-        <v>0.378</v>
+        <v>0.38900000000000001</v>
       </c>
       <c r="L33" s="3">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M33" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N33" s="3">
         <v>0</v>
@@ -2916,8 +2922,8 @@
       <c r="O33" s="3">
         <v>0</v>
       </c>
-      <c r="P33" s="6" t="s">
-        <v>125</v>
+      <c r="P33" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -2928,155 +2934,155 @@
         <v>1610612746</v>
       </c>
       <c r="C34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1978</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1983</v>
+      </c>
+      <c r="G34" s="3">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3">
+        <v>492</v>
+      </c>
+      <c r="I34" s="3">
+        <v>186</v>
+      </c>
+      <c r="J34" s="3">
+        <v>306</v>
+      </c>
+      <c r="K34" s="3">
+        <v>0.378</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3">
+        <v>0</v>
+      </c>
+      <c r="O34" s="3">
+        <v>0</v>
+      </c>
+      <c r="P34" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1610612746</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D35" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E35" s="3">
         <v>1970</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F35" s="3">
         <v>1977</v>
       </c>
-      <c r="G34" s="3">
+      <c r="G35" s="3">
         <v>8</v>
       </c>
-      <c r="H34" s="3">
+      <c r="H35" s="3">
         <v>656</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I35" s="3">
         <v>259</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J35" s="3">
         <v>397</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K35" s="3">
         <v>0.39400000000000002</v>
       </c>
-      <c r="L34" s="3">
+      <c r="L35" s="3">
         <v>3</v>
       </c>
-      <c r="M34" s="3">
-        <v>0</v>
-      </c>
-      <c r="N34" s="3">
-        <v>0</v>
-      </c>
-      <c r="O34" s="3">
-        <v>0</v>
-      </c>
-      <c r="P34" s="3" t="s">
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3">
+        <v>0</v>
+      </c>
+      <c r="O35" s="3">
+        <v>0</v>
+      </c>
+      <c r="P35" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:21">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:21">
+      <c r="A36" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B36" s="4">
         <v>1610612747</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E36" s="4">
         <v>1948</v>
       </c>
-      <c r="F35" s="4">
+      <c r="F36" s="4">
         <v>2016</v>
       </c>
-      <c r="G35" s="4">
+      <c r="G36" s="4">
         <v>69</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H36" s="4">
         <v>5380</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I36" s="4">
         <v>3241</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J36" s="4">
         <v>2139</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K36" s="4">
         <v>0.60199999999999998</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L36" s="4">
         <v>60</v>
       </c>
-      <c r="M35" s="4">
+      <c r="M36" s="4">
         <v>34</v>
       </c>
-      <c r="N35" s="4">
+      <c r="N36" s="4">
         <v>18</v>
       </c>
-      <c r="O35" s="4">
+      <c r="O36" s="4">
         <v>16</v>
       </c>
-      <c r="P35" s="4" t="s">
+      <c r="P36" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Q35" s="3" t="s">
+      <c r="Q36" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="R35" s="3" t="s">
+      <c r="R36" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="S35" s="3" t="s">
+      <c r="S36" s="3" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
-      <c r="A36" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B36" s="3">
-        <v>1610612747</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E36" s="3">
-        <v>1960</v>
-      </c>
-      <c r="F36" s="3">
-        <v>2016</v>
-      </c>
-      <c r="G36" s="3">
-        <v>57</v>
-      </c>
-      <c r="H36" s="3">
-        <v>4538</v>
-      </c>
-      <c r="I36" s="3">
-        <v>2782</v>
-      </c>
-      <c r="J36" s="3">
-        <v>1756</v>
-      </c>
-      <c r="K36" s="3">
-        <v>0.61299999999999999</v>
-      </c>
-      <c r="L36" s="3">
-        <v>49</v>
-      </c>
-      <c r="M36" s="3">
-        <v>29</v>
-      </c>
-      <c r="N36" s="3">
-        <v>18</v>
-      </c>
-      <c r="O36" s="3">
-        <v>11</v>
-      </c>
-      <c r="P36" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -3087,158 +3093,158 @@
         <v>1610612747</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E37" s="3">
+        <v>1960</v>
+      </c>
+      <c r="F37" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G37" s="3">
+        <v>57</v>
+      </c>
+      <c r="H37" s="3">
+        <v>4538</v>
+      </c>
+      <c r="I37" s="3">
+        <v>2782</v>
+      </c>
+      <c r="J37" s="3">
+        <v>1756</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="L37" s="3">
+        <v>49</v>
+      </c>
+      <c r="M37" s="3">
+        <v>29</v>
+      </c>
+      <c r="N37" s="3">
+        <v>18</v>
+      </c>
+      <c r="O37" s="3">
+        <v>11</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1610612747</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" s="3">
         <v>1948</v>
       </c>
-      <c r="F37" s="3">
+      <c r="F38" s="3">
         <v>1959</v>
       </c>
-      <c r="G37" s="3">
+      <c r="G38" s="3">
         <v>12</v>
       </c>
-      <c r="H37" s="3">
+      <c r="H38" s="3">
         <v>842</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I38" s="3">
         <v>459</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J38" s="3">
         <v>383</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K38" s="3">
         <v>0.54500000000000004</v>
       </c>
-      <c r="L37" s="3">
+      <c r="L38" s="3">
         <v>11</v>
       </c>
-      <c r="M37" s="3">
+      <c r="M38" s="3">
         <v>5</v>
       </c>
-      <c r="N37" s="3">
-        <v>0</v>
-      </c>
-      <c r="O37" s="3">
+      <c r="N38" s="3">
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
         <v>5</v>
       </c>
-      <c r="P37" s="6" t="s">
+      <c r="P38" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:21">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:21">
+      <c r="A39" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B39" s="4">
         <v>1610612763</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E39" s="4">
         <v>1995</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F39" s="4">
         <v>2016</v>
       </c>
-      <c r="G38" s="4">
+      <c r="G39" s="4">
         <v>22</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H39" s="4">
         <v>1682</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I39" s="4">
         <v>698</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J39" s="4">
         <v>984</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K39" s="4">
         <v>0.41399999999999998</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L39" s="4">
         <v>9</v>
       </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
-        <v>0</v>
-      </c>
-      <c r="O38" s="4">
-        <v>0</v>
-      </c>
-      <c r="P38" s="4" t="s">
+      <c r="M39" s="4">
+        <v>0</v>
+      </c>
+      <c r="N39" s="4">
+        <v>0</v>
+      </c>
+      <c r="O39" s="4">
+        <v>0</v>
+      </c>
+      <c r="P39" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="Q38" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="R38" s="3" t="s">
+      <c r="R39" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="S38" s="3" t="s">
+      <c r="S39" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="T38" s="3" t="s">
+      <c r="T39" s="3" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
-      <c r="A39" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B39" s="3">
-        <v>1610612763</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="3">
-        <v>2001</v>
-      </c>
-      <c r="F39" s="3">
-        <v>2016</v>
-      </c>
-      <c r="G39" s="3">
-        <v>16</v>
-      </c>
-      <c r="H39" s="3">
-        <v>1222</v>
-      </c>
-      <c r="I39" s="3">
-        <v>597</v>
-      </c>
-      <c r="J39" s="3">
-        <v>625</v>
-      </c>
-      <c r="K39" s="3">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="L39" s="3">
-        <v>9</v>
-      </c>
-      <c r="M39" s="3">
-        <v>0</v>
-      </c>
-      <c r="N39" s="3">
-        <v>0</v>
-      </c>
-      <c r="O39" s="3">
-        <v>0</v>
-      </c>
-      <c r="P39" s="3" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -3249,108 +3255,96 @@
         <v>1610612763</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>56</v>
       </c>
       <c r="E40" s="3">
+        <v>2001</v>
+      </c>
+      <c r="F40" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G40" s="3">
+        <v>16</v>
+      </c>
+      <c r="H40" s="3">
+        <v>1222</v>
+      </c>
+      <c r="I40" s="3">
+        <v>597</v>
+      </c>
+      <c r="J40" s="3">
+        <v>625</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="L40" s="3">
+        <v>9</v>
+      </c>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+      <c r="N40" s="3">
+        <v>0</v>
+      </c>
+      <c r="O40" s="3">
+        <v>0</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21">
+      <c r="A41" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1610612763</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" s="3">
         <v>1995</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F41" s="3">
         <v>2000</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G41" s="3">
         <v>6</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H41" s="3">
         <v>460</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I41" s="3">
         <v>101</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J41" s="3">
         <v>359</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K41" s="3">
         <v>0.219</v>
       </c>
-      <c r="L40" s="3">
-        <v>0</v>
-      </c>
-      <c r="M40" s="3">
-        <v>0</v>
-      </c>
-      <c r="N40" s="3">
-        <v>0</v>
-      </c>
-      <c r="O40" s="3">
-        <v>0</v>
-      </c>
-      <c r="P40" s="6" t="s">
+      <c r="L41" s="3">
+        <v>0</v>
+      </c>
+      <c r="M41" s="3">
+        <v>0</v>
+      </c>
+      <c r="N41" s="3">
+        <v>0</v>
+      </c>
+      <c r="O41" s="3">
+        <v>0</v>
+      </c>
+      <c r="P41" s="6" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
-      <c r="A41" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B41" s="4">
-        <v>1610612748</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="4">
-        <v>1988</v>
-      </c>
-      <c r="F41" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G41" s="4">
-        <v>29</v>
-      </c>
-      <c r="H41" s="4">
-        <v>2254</v>
-      </c>
-      <c r="I41" s="4">
-        <v>1172</v>
-      </c>
-      <c r="J41" s="4">
-        <v>1082</v>
-      </c>
-      <c r="K41" s="4">
-        <v>0.51900000000000002</v>
-      </c>
-      <c r="L41" s="4">
-        <v>19</v>
-      </c>
-      <c r="M41" s="4">
-        <v>12</v>
-      </c>
-      <c r="N41" s="4">
-        <v>5</v>
-      </c>
-      <c r="O41" s="4">
-        <v>3</v>
-      </c>
-      <c r="P41" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="Q41" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="R41" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="S41" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="T41" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -3358,63 +3352,60 @@
         <v>177</v>
       </c>
       <c r="B42" s="4">
-        <v>1610612749</v>
+        <v>1610612748</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E42" s="4">
-        <v>1968</v>
+        <v>1988</v>
       </c>
       <c r="F42" s="4">
         <v>2016</v>
       </c>
       <c r="G42" s="4">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="H42" s="4">
-        <v>3895</v>
+        <v>2254</v>
       </c>
       <c r="I42" s="4">
-        <v>1987</v>
+        <v>1172</v>
       </c>
       <c r="J42" s="4">
-        <v>1908</v>
+        <v>1082</v>
       </c>
       <c r="K42" s="4">
-        <v>0.51</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="L42" s="4">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="M42" s="4">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N42" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O42" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P42" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="Q42" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="R42" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="U42" s="3" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3423,58 +3414,58 @@
         <v>177</v>
       </c>
       <c r="B43" s="4">
-        <v>1610612750</v>
+        <v>1610612749</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E43" s="4">
-        <v>1989</v>
+        <v>1968</v>
       </c>
       <c r="F43" s="4">
         <v>2016</v>
       </c>
       <c r="G43" s="4">
+        <v>49</v>
+      </c>
+      <c r="H43" s="4">
+        <v>3895</v>
+      </c>
+      <c r="I43" s="4">
+        <v>1987</v>
+      </c>
+      <c r="J43" s="4">
+        <v>1908</v>
+      </c>
+      <c r="K43" s="4">
+        <v>0.51</v>
+      </c>
+      <c r="L43" s="4">
         <v>28</v>
       </c>
-      <c r="H43" s="4">
-        <v>2172</v>
-      </c>
-      <c r="I43" s="4">
-        <v>848</v>
-      </c>
-      <c r="J43" s="4">
-        <v>1324</v>
-      </c>
-      <c r="K43" s="4">
-        <v>0.39</v>
-      </c>
-      <c r="L43" s="4">
-        <v>8</v>
-      </c>
       <c r="M43" s="4">
+        <v>13</v>
+      </c>
+      <c r="N43" s="4">
+        <v>2</v>
+      </c>
+      <c r="O43" s="4">
         <v>1</v>
       </c>
-      <c r="N43" s="4">
-        <v>0</v>
-      </c>
-      <c r="O43" s="4">
-        <v>0</v>
-      </c>
       <c r="P43" s="4" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="Q43" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="R43" s="3" t="s">
-        <v>180</v>
+        <v>201</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="T43" s="3" t="s">
         <v>164</v>
@@ -3488,37 +3479,37 @@
         <v>177</v>
       </c>
       <c r="B44" s="4">
-        <v>1610612740</v>
+        <v>1610612750</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E44" s="4">
-        <v>2002</v>
+        <v>1989</v>
       </c>
       <c r="F44" s="4">
         <v>2016</v>
       </c>
       <c r="G44" s="4">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="H44" s="4">
-        <v>1140</v>
+        <v>2172</v>
       </c>
       <c r="I44" s="4">
-        <v>528</v>
+        <v>848</v>
       </c>
       <c r="J44" s="4">
-        <v>612</v>
+        <v>1324</v>
       </c>
       <c r="K44" s="4">
-        <v>0.46300000000000002</v>
+        <v>0.39</v>
       </c>
       <c r="L44" s="4">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="M44" s="4">
         <v>1</v>
@@ -3530,69 +3521,84 @@
         <v>0</v>
       </c>
       <c r="P44" s="4" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="Q44" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="R44" s="3" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="T44" s="3" t="s">
         <v>164</v>
       </c>
+      <c r="U44" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="45" spans="1:21">
-      <c r="A45" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B45" s="3">
+      <c r="A45" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="4">
         <v>1610612740</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="3">
-        <v>2013</v>
-      </c>
-      <c r="F45" s="3">
+      <c r="E45" s="4">
+        <v>2002</v>
+      </c>
+      <c r="F45" s="4">
         <v>2016</v>
       </c>
-      <c r="G45" s="3">
-        <v>4</v>
-      </c>
-      <c r="H45" s="3">
-        <v>254</v>
-      </c>
-      <c r="I45" s="3">
-        <v>109</v>
-      </c>
-      <c r="J45" s="3">
-        <v>145</v>
-      </c>
-      <c r="K45" s="3">
-        <v>0.42899999999999999</v>
-      </c>
-      <c r="L45" s="3">
+      <c r="G45" s="4">
+        <v>15</v>
+      </c>
+      <c r="H45" s="4">
+        <v>1140</v>
+      </c>
+      <c r="I45" s="4">
+        <v>528</v>
+      </c>
+      <c r="J45" s="4">
+        <v>612</v>
+      </c>
+      <c r="K45" s="4">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="L45" s="4">
+        <v>6</v>
+      </c>
+      <c r="M45" s="4">
         <v>1</v>
       </c>
-      <c r="M45" s="3">
-        <v>0</v>
-      </c>
-      <c r="N45" s="3">
-        <v>0</v>
-      </c>
-      <c r="O45" s="3">
-        <v>0</v>
-      </c>
-      <c r="P45" s="3" t="s">
+      <c r="N45" s="4">
+        <v>0</v>
+      </c>
+      <c r="O45" s="4">
+        <v>0</v>
+      </c>
+      <c r="P45" s="4" t="s">
         <v>134</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="T45" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -3606,34 +3612,34 @@
         <v>63</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E46" s="3">
-        <v>2002</v>
+        <v>2013</v>
       </c>
       <c r="F46" s="3">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="G46" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H46" s="3">
-        <v>722</v>
+        <v>254</v>
       </c>
       <c r="I46" s="3">
-        <v>342</v>
+        <v>109</v>
       </c>
       <c r="J46" s="3">
-        <v>380</v>
+        <v>145</v>
       </c>
       <c r="K46" s="3">
-        <v>0.47299999999999998</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="L46" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M46" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N46" s="3">
         <v>0</v>
@@ -3642,7 +3648,7 @@
         <v>0</v>
       </c>
       <c r="P46" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -3653,108 +3659,96 @@
         <v>1610612740</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E47" s="3">
+        <v>2002</v>
+      </c>
+      <c r="F47" s="3">
+        <v>2012</v>
+      </c>
+      <c r="G47" s="3">
+        <v>9</v>
+      </c>
+      <c r="H47" s="3">
+        <v>722</v>
+      </c>
+      <c r="I47" s="3">
+        <v>342</v>
+      </c>
+      <c r="J47" s="3">
+        <v>380</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="L47" s="3">
+        <v>5</v>
+      </c>
+      <c r="M47" s="3">
+        <v>1</v>
+      </c>
+      <c r="N47" s="3">
+        <v>0</v>
+      </c>
+      <c r="O47" s="3">
+        <v>0</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1610612740</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="3">
         <v>2005</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F48" s="3">
         <v>2006</v>
       </c>
-      <c r="G47" s="3">
+      <c r="G48" s="3">
         <v>2</v>
       </c>
-      <c r="H47" s="3">
+      <c r="H48" s="3">
         <v>164</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I48" s="3">
         <v>77</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J48" s="3">
         <v>87</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K48" s="3">
         <v>0.46899999999999997</v>
       </c>
-      <c r="L47" s="3">
-        <v>0</v>
-      </c>
-      <c r="M47" s="3">
-        <v>0</v>
-      </c>
-      <c r="N47" s="3">
-        <v>0</v>
-      </c>
-      <c r="O47" s="3">
-        <v>0</v>
-      </c>
-      <c r="P47" s="3" t="s">
+      <c r="L48" s="3">
+        <v>0</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+      <c r="N48" s="3">
+        <v>0</v>
+      </c>
+      <c r="O48" s="3">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
-      <c r="A48" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B48" s="4">
-        <v>1610612752</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E48" s="4">
-        <v>1946</v>
-      </c>
-      <c r="F48" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G48" s="4">
-        <v>71</v>
-      </c>
-      <c r="H48" s="4">
-        <v>5482</v>
-      </c>
-      <c r="I48" s="4">
-        <v>2703</v>
-      </c>
-      <c r="J48" s="4">
-        <v>2779</v>
-      </c>
-      <c r="K48" s="4">
-        <v>0.49299999999999999</v>
-      </c>
-      <c r="L48" s="4">
-        <v>41</v>
-      </c>
-      <c r="M48" s="4">
-        <v>9</v>
-      </c>
-      <c r="N48" s="4">
-        <v>4</v>
-      </c>
-      <c r="O48" s="4">
-        <v>2</v>
-      </c>
-      <c r="P48" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q48" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="R48" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="S48" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="T48" s="3" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -3762,111 +3756,123 @@
         <v>177</v>
       </c>
       <c r="B49" s="4">
-        <v>1610612760</v>
+        <v>1610612752</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E49" s="4">
-        <v>1967</v>
+        <v>1946</v>
       </c>
       <c r="F49" s="4">
         <v>2016</v>
       </c>
       <c r="G49" s="4">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="H49" s="4">
-        <v>3977</v>
+        <v>5482</v>
       </c>
       <c r="I49" s="4">
-        <v>2145</v>
+        <v>2703</v>
       </c>
       <c r="J49" s="4">
-        <v>1832</v>
+        <v>2779</v>
       </c>
       <c r="K49" s="4">
-        <v>0.53900000000000003</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="L49" s="4">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="M49" s="4">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N49" s="4">
         <v>4</v>
       </c>
       <c r="O49" s="4">
+        <v>2</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="T49" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21">
+      <c r="A50" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B50" s="4">
+        <v>1610612760</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50" s="4">
+        <v>1967</v>
+      </c>
+      <c r="F50" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G50" s="4">
+        <v>50</v>
+      </c>
+      <c r="H50" s="4">
+        <v>3977</v>
+      </c>
+      <c r="I50" s="4">
+        <v>2145</v>
+      </c>
+      <c r="J50" s="4">
+        <v>1832</v>
+      </c>
+      <c r="K50" s="4">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="L50" s="4">
+        <v>28</v>
+      </c>
+      <c r="M50" s="4">
+        <v>12</v>
+      </c>
+      <c r="N50" s="4">
+        <v>4</v>
+      </c>
+      <c r="O50" s="4">
         <v>1</v>
       </c>
-      <c r="P49" s="4" t="s">
+      <c r="P50" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="Q49" s="3" t="s">
+      <c r="Q50" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="R49" s="3" t="s">
+      <c r="R50" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="S49" s="3" t="s">
+      <c r="S50" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="T49" s="3" t="s">
+      <c r="T50" s="3" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
-      <c r="A50" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B50" s="3">
-        <v>1610612760</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" s="3">
-        <v>2008</v>
-      </c>
-      <c r="F50" s="3">
-        <v>2016</v>
-      </c>
-      <c r="G50" s="3">
-        <v>9</v>
-      </c>
-      <c r="H50" s="3">
-        <v>647</v>
-      </c>
-      <c r="I50" s="3">
-        <v>400</v>
-      </c>
-      <c r="J50" s="3">
-        <v>247</v>
-      </c>
-      <c r="K50" s="3">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="L50" s="3">
-        <v>6</v>
-      </c>
-      <c r="M50" s="3">
-        <v>6</v>
-      </c>
-      <c r="N50" s="3">
-        <v>1</v>
-      </c>
-      <c r="O50" s="3">
-        <v>0</v>
-      </c>
-      <c r="P50" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -3877,108 +3883,96 @@
         <v>1610612760</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E51" s="3">
-        <v>1967</v>
+        <v>2008</v>
       </c>
       <c r="F51" s="3">
-        <v>2007</v>
+        <v>2016</v>
       </c>
       <c r="G51" s="3">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="H51" s="3">
-        <v>3330</v>
+        <v>647</v>
       </c>
       <c r="I51" s="3">
-        <v>1745</v>
+        <v>400</v>
       </c>
       <c r="J51" s="3">
-        <v>1585</v>
+        <v>247</v>
       </c>
       <c r="K51" s="3">
-        <v>0.52400000000000002</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="L51" s="3">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="M51" s="3">
         <v>6</v>
       </c>
       <c r="N51" s="3">
+        <v>1</v>
+      </c>
+      <c r="O51" s="3">
+        <v>0</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21">
+      <c r="A52" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1610612760</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1967</v>
+      </c>
+      <c r="F52" s="3">
+        <v>2007</v>
+      </c>
+      <c r="G52" s="3">
+        <v>41</v>
+      </c>
+      <c r="H52" s="3">
+        <v>3330</v>
+      </c>
+      <c r="I52" s="3">
+        <v>1745</v>
+      </c>
+      <c r="J52" s="3">
+        <v>1585</v>
+      </c>
+      <c r="K52" s="3">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="L52" s="3">
+        <v>22</v>
+      </c>
+      <c r="M52" s="3">
+        <v>6</v>
+      </c>
+      <c r="N52" s="3">
         <v>3</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O52" s="3">
         <v>1</v>
       </c>
-      <c r="P51" s="3" t="s">
+      <c r="P52" s="3" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
-      <c r="A52" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B52" s="4">
-        <v>1610612753</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" s="4">
-        <v>1989</v>
-      </c>
-      <c r="F52" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G52" s="4">
-        <v>28</v>
-      </c>
-      <c r="H52" s="4">
-        <v>2173</v>
-      </c>
-      <c r="I52" s="4">
-        <v>1065</v>
-      </c>
-      <c r="J52" s="4">
-        <v>1108</v>
-      </c>
-      <c r="K52" s="4">
-        <v>0.49</v>
-      </c>
-      <c r="L52" s="4">
-        <v>14</v>
-      </c>
-      <c r="M52" s="4">
-        <v>6</v>
-      </c>
-      <c r="N52" s="4">
-        <v>2</v>
-      </c>
-      <c r="O52" s="4">
-        <v>0</v>
-      </c>
-      <c r="P52" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q52" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="R52" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="S52" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="T52" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -3986,108 +3980,120 @@
         <v>177</v>
       </c>
       <c r="B53" s="4">
-        <v>1610612755</v>
+        <v>1610612753</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E53" s="4">
-        <v>1949</v>
+        <v>1989</v>
       </c>
       <c r="F53" s="4">
         <v>2016</v>
       </c>
       <c r="G53" s="4">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="H53" s="4">
-        <v>5311</v>
+        <v>2173</v>
       </c>
       <c r="I53" s="4">
-        <v>2727</v>
+        <v>1065</v>
       </c>
       <c r="J53" s="4">
-        <v>2584</v>
+        <v>1108</v>
       </c>
       <c r="K53" s="4">
-        <v>0.51300000000000001</v>
+        <v>0.49</v>
       </c>
       <c r="L53" s="4">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="M53" s="4">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N53" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O53" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="P53" s="4" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="R53" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="S53" s="3" t="s">
         <v>164</v>
       </c>
+      <c r="T53" s="3" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="54" spans="1:21">
-      <c r="A54" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B54" s="3">
+      <c r="A54" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B54" s="4">
         <v>1610612755</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E54" s="3">
-        <v>1963</v>
-      </c>
-      <c r="F54" s="3">
+      <c r="E54" s="4">
+        <v>1949</v>
+      </c>
+      <c r="F54" s="4">
         <v>2016</v>
       </c>
-      <c r="G54" s="3">
-        <v>54</v>
-      </c>
-      <c r="H54" s="3">
-        <v>4297</v>
-      </c>
-      <c r="I54" s="3">
-        <v>2150</v>
-      </c>
-      <c r="J54" s="3">
-        <v>2147</v>
-      </c>
-      <c r="K54" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="L54" s="3">
-        <v>33</v>
-      </c>
-      <c r="M54" s="3">
-        <v>9</v>
-      </c>
-      <c r="N54" s="3">
+      <c r="G54" s="4">
+        <v>68</v>
+      </c>
+      <c r="H54" s="4">
+        <v>5311</v>
+      </c>
+      <c r="I54" s="4">
+        <v>2727</v>
+      </c>
+      <c r="J54" s="4">
+        <v>2584</v>
+      </c>
+      <c r="K54" s="4">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="L54" s="4">
+        <v>47</v>
+      </c>
+      <c r="M54" s="4">
+        <v>12</v>
+      </c>
+      <c r="N54" s="4">
         <v>5</v>
       </c>
-      <c r="O54" s="3">
-        <v>2</v>
-      </c>
-      <c r="P54" s="3" t="s">
+      <c r="O54" s="4">
+        <v>3</v>
+      </c>
+      <c r="P54" s="4" t="s">
         <v>112</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -4098,111 +4104,96 @@
         <v>1610612755</v>
       </c>
       <c r="C55" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1963</v>
+      </c>
+      <c r="F55" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G55" s="3">
+        <v>54</v>
+      </c>
+      <c r="H55" s="3">
+        <v>4297</v>
+      </c>
+      <c r="I55" s="3">
+        <v>2150</v>
+      </c>
+      <c r="J55" s="3">
+        <v>2147</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="L55" s="3">
+        <v>33</v>
+      </c>
+      <c r="M55" s="3">
+        <v>9</v>
+      </c>
+      <c r="N55" s="3">
+        <v>5</v>
+      </c>
+      <c r="O55" s="3">
+        <v>2</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21">
+      <c r="A56" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1610612755</v>
+      </c>
+      <c r="C56" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E55" s="3">
+      <c r="E56" s="3">
         <v>1949</v>
       </c>
-      <c r="F55" s="3">
+      <c r="F56" s="3">
         <v>1962</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G56" s="3">
         <v>14</v>
       </c>
-      <c r="H55" s="3">
+      <c r="H56" s="3">
         <v>1014</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I56" s="3">
         <v>577</v>
       </c>
-      <c r="J55" s="3">
+      <c r="J56" s="3">
         <v>437</v>
       </c>
-      <c r="K55" s="3">
+      <c r="K56" s="3">
         <v>0.56899999999999995</v>
       </c>
-      <c r="L55" s="3">
+      <c r="L56" s="3">
         <v>14</v>
       </c>
-      <c r="M55" s="3">
+      <c r="M56" s="3">
         <v>3</v>
       </c>
-      <c r="N55" s="3">
-        <v>0</v>
-      </c>
-      <c r="O55" s="3">
+      <c r="N56" s="3">
+        <v>0</v>
+      </c>
+      <c r="O56" s="3">
         <v>1</v>
       </c>
-      <c r="P55" s="3" t="s">
+      <c r="P56" s="3" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
-      <c r="A56" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B56" s="4">
-        <v>1610612756</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E56" s="4">
-        <v>1968</v>
-      </c>
-      <c r="F56" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G56" s="4">
-        <v>49</v>
-      </c>
-      <c r="H56" s="4">
-        <v>3896</v>
-      </c>
-      <c r="I56" s="4">
-        <v>2124</v>
-      </c>
-      <c r="J56" s="4">
-        <v>1772</v>
-      </c>
-      <c r="K56" s="4">
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="L56" s="4">
-        <v>29</v>
-      </c>
-      <c r="M56" s="4">
-        <v>6</v>
-      </c>
-      <c r="N56" s="4">
-        <v>2</v>
-      </c>
-      <c r="O56" s="4">
-        <v>0</v>
-      </c>
-      <c r="P56" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="Q56" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="R56" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="S56" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="T56" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="U56" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -4210,60 +4201,63 @@
         <v>177</v>
       </c>
       <c r="B57" s="4">
-        <v>1610612757</v>
+        <v>1610612756</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E57" s="4">
-        <v>1970</v>
+        <v>1968</v>
       </c>
       <c r="F57" s="4">
         <v>2016</v>
       </c>
       <c r="G57" s="4">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H57" s="4">
-        <v>3732</v>
+        <v>3896</v>
       </c>
       <c r="I57" s="4">
-        <v>1996</v>
+        <v>2124</v>
       </c>
       <c r="J57" s="4">
-        <v>1736</v>
+        <v>1772</v>
       </c>
       <c r="K57" s="4">
-        <v>0.53400000000000003</v>
+        <v>0.54500000000000004</v>
       </c>
       <c r="L57" s="4">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M57" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N57" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O57" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P57" s="4" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="Q57" s="3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="R57" s="3" t="s">
-        <v>214</v>
+        <v>169</v>
       </c>
       <c r="S57" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="T57" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="T57" s="3" t="s">
+      <c r="U57" s="3" t="s">
         <v>165</v>
       </c>
     </row>
@@ -4272,55 +4266,55 @@
         <v>177</v>
       </c>
       <c r="B58" s="4">
-        <v>1610612758</v>
+        <v>1610612757</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E58" s="4">
-        <v>1948</v>
+        <v>1970</v>
       </c>
       <c r="F58" s="4">
         <v>2016</v>
       </c>
       <c r="G58" s="4">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="H58" s="4">
-        <v>5379</v>
+        <v>3732</v>
       </c>
       <c r="I58" s="4">
-        <v>2468</v>
+        <v>1996</v>
       </c>
       <c r="J58" s="4">
-        <v>2911</v>
+        <v>1736</v>
       </c>
       <c r="K58" s="4">
-        <v>0.45800000000000002</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="L58" s="4">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M58" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N58" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O58" s="4">
         <v>1</v>
       </c>
       <c r="P58" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q58" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="R58" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="S58" s="3" t="s">
         <v>164</v>
@@ -4330,53 +4324,65 @@
       </c>
     </row>
     <row r="59" spans="1:21">
-      <c r="A59" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B59" s="3">
+      <c r="A59" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" s="4">
         <v>1610612758</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E59" s="3">
-        <v>1985</v>
-      </c>
-      <c r="F59" s="3">
+      <c r="E59" s="4">
+        <v>1948</v>
+      </c>
+      <c r="F59" s="4">
         <v>2016</v>
       </c>
-      <c r="G59" s="3">
-        <v>32</v>
-      </c>
-      <c r="H59" s="3">
-        <v>2503</v>
-      </c>
-      <c r="I59" s="3">
-        <v>1062</v>
-      </c>
-      <c r="J59" s="3">
-        <v>1441</v>
-      </c>
-      <c r="K59" s="3">
-        <v>0.42399999999999999</v>
-      </c>
-      <c r="L59" s="3">
-        <v>10</v>
-      </c>
-      <c r="M59" s="3">
-        <v>2</v>
-      </c>
-      <c r="N59" s="3">
-        <v>0</v>
-      </c>
-      <c r="O59" s="3">
-        <v>0</v>
-      </c>
-      <c r="P59" s="3" t="s">
+      <c r="G59" s="4">
+        <v>69</v>
+      </c>
+      <c r="H59" s="4">
+        <v>5379</v>
+      </c>
+      <c r="I59" s="4">
+        <v>2468</v>
+      </c>
+      <c r="J59" s="4">
+        <v>2911</v>
+      </c>
+      <c r="K59" s="4">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="L59" s="4">
+        <v>29</v>
+      </c>
+      <c r="M59" s="4">
+        <v>6</v>
+      </c>
+      <c r="N59" s="4">
+        <v>0</v>
+      </c>
+      <c r="O59" s="4">
+        <v>1</v>
+      </c>
+      <c r="P59" s="4" t="s">
         <v>142</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="R59" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="T59" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -4387,37 +4393,37 @@
         <v>1610612758</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E60" s="3">
-        <v>1975</v>
+        <v>1985</v>
       </c>
       <c r="F60" s="3">
-        <v>1984</v>
+        <v>2016</v>
       </c>
       <c r="G60" s="3">
+        <v>32</v>
+      </c>
+      <c r="H60" s="3">
+        <v>2503</v>
+      </c>
+      <c r="I60" s="3">
+        <v>1062</v>
+      </c>
+      <c r="J60" s="3">
+        <v>1441</v>
+      </c>
+      <c r="K60" s="3">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="L60" s="3">
         <v>10</v>
       </c>
-      <c r="H60" s="3">
-        <v>820</v>
-      </c>
-      <c r="I60" s="3">
-        <v>381</v>
-      </c>
-      <c r="J60" s="3">
-        <v>439</v>
-      </c>
-      <c r="K60" s="3">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="L60" s="3">
-        <v>4</v>
-      </c>
       <c r="M60" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N60" s="3">
         <v>0</v>
@@ -4426,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -4437,37 +4443,37 @@
         <v>1610612758</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D61" s="3" t="s">
         <v>81</v>
       </c>
       <c r="E61" s="3">
-        <v>1972</v>
+        <v>1975</v>
       </c>
       <c r="F61" s="3">
-        <v>1974</v>
+        <v>1984</v>
       </c>
       <c r="G61" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="H61" s="3">
-        <v>246</v>
+        <v>820</v>
       </c>
       <c r="I61" s="3">
-        <v>113</v>
+        <v>381</v>
       </c>
       <c r="J61" s="3">
-        <v>133</v>
+        <v>439</v>
       </c>
       <c r="K61" s="3">
-        <v>0.45900000000000002</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="L61" s="3">
+        <v>4</v>
+      </c>
+      <c r="M61" s="3">
         <v>1</v>
-      </c>
-      <c r="M61" s="3">
-        <v>0</v>
       </c>
       <c r="N61" s="3">
         <v>0</v>
@@ -4487,34 +4493,34 @@
         <v>1610612758</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E62" s="3">
-        <v>1957</v>
+        <v>1972</v>
       </c>
       <c r="F62" s="3">
-        <v>1971</v>
+        <v>1974</v>
       </c>
       <c r="G62" s="3">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H62" s="3">
-        <v>1189</v>
+        <v>246</v>
       </c>
       <c r="I62" s="3">
-        <v>555</v>
+        <v>113</v>
       </c>
       <c r="J62" s="3">
-        <v>634</v>
+        <v>133</v>
       </c>
       <c r="K62" s="3">
-        <v>0.46600000000000003</v>
+        <v>0.45900000000000002</v>
       </c>
       <c r="L62" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="M62" s="3">
         <v>0</v>
@@ -4526,7 +4532,7 @@
         <v>0</v>
       </c>
       <c r="P62" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -4537,105 +4543,96 @@
         <v>1610612758</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>85</v>
       </c>
       <c r="E63" s="3">
-        <v>1948</v>
+        <v>1957</v>
       </c>
       <c r="F63" s="3">
-        <v>1956</v>
+        <v>1971</v>
       </c>
       <c r="G63" s="3">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="H63" s="3">
-        <v>621</v>
+        <v>1189</v>
       </c>
       <c r="I63" s="3">
-        <v>357</v>
+        <v>555</v>
       </c>
       <c r="J63" s="3">
-        <v>264</v>
+        <v>634</v>
       </c>
       <c r="K63" s="3">
-        <v>0.57399999999999995</v>
+        <v>0.46600000000000003</v>
       </c>
       <c r="L63" s="3">
         <v>7</v>
       </c>
       <c r="M63" s="3">
+        <v>0</v>
+      </c>
+      <c r="N63" s="3">
+        <v>0</v>
+      </c>
+      <c r="O63" s="3">
+        <v>0</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21">
+      <c r="A64" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1610612758</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1948</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1956</v>
+      </c>
+      <c r="G64" s="3">
+        <v>9</v>
+      </c>
+      <c r="H64" s="3">
+        <v>621</v>
+      </c>
+      <c r="I64" s="3">
+        <v>357</v>
+      </c>
+      <c r="J64" s="3">
+        <v>264</v>
+      </c>
+      <c r="K64" s="3">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="L64" s="3">
+        <v>7</v>
+      </c>
+      <c r="M64" s="3">
         <v>3</v>
       </c>
-      <c r="N63" s="3">
-        <v>0</v>
-      </c>
-      <c r="O63" s="3">
+      <c r="N64" s="3">
+        <v>0</v>
+      </c>
+      <c r="O64" s="3">
         <v>1</v>
       </c>
-      <c r="P63" s="3" t="s">
+      <c r="P64" s="3" t="s">
         <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21">
-      <c r="A64" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B64" s="4">
-        <v>1610612759</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" s="4">
-        <v>1976</v>
-      </c>
-      <c r="F64" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G64" s="4">
-        <v>41</v>
-      </c>
-      <c r="H64" s="4">
-        <v>3239</v>
-      </c>
-      <c r="I64" s="4">
-        <v>2011</v>
-      </c>
-      <c r="J64" s="4">
-        <v>1228</v>
-      </c>
-      <c r="K64" s="4">
-        <v>0.62</v>
-      </c>
-      <c r="L64" s="4">
-        <v>36</v>
-      </c>
-      <c r="M64" s="4">
-        <v>22</v>
-      </c>
-      <c r="N64" s="4">
-        <v>6</v>
-      </c>
-      <c r="O64" s="4">
-        <v>5</v>
-      </c>
-      <c r="P64" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q64" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="R64" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="S64" s="3" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="65" spans="1:20">
@@ -4643,58 +4640,58 @@
         <v>177</v>
       </c>
       <c r="B65" s="4">
-        <v>1610612761</v>
+        <v>1610612759</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E65" s="4">
-        <v>1995</v>
+        <v>1976</v>
       </c>
       <c r="F65" s="4">
         <v>2016</v>
       </c>
       <c r="G65" s="4">
+        <v>41</v>
+      </c>
+      <c r="H65" s="4">
+        <v>3239</v>
+      </c>
+      <c r="I65" s="4">
+        <v>2011</v>
+      </c>
+      <c r="J65" s="4">
+        <v>1228</v>
+      </c>
+      <c r="K65" s="4">
+        <v>0.62</v>
+      </c>
+      <c r="L65" s="4">
+        <v>36</v>
+      </c>
+      <c r="M65" s="4">
         <v>22</v>
       </c>
-      <c r="H65" s="4">
-        <v>1680</v>
-      </c>
-      <c r="I65" s="4">
-        <v>738</v>
-      </c>
-      <c r="J65" s="4">
-        <v>942</v>
-      </c>
-      <c r="K65" s="4">
-        <v>0.439</v>
-      </c>
-      <c r="L65" s="4">
-        <v>8</v>
-      </c>
-      <c r="M65" s="4">
+      <c r="N65" s="4">
+        <v>6</v>
+      </c>
+      <c r="O65" s="4">
         <v>5</v>
       </c>
-      <c r="N65" s="4">
-        <v>0</v>
-      </c>
-      <c r="O65" s="4">
-        <v>0</v>
-      </c>
       <c r="P65" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Q65" s="3" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="R65" s="3" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:20">
@@ -4702,223 +4699,229 @@
         <v>177</v>
       </c>
       <c r="B66" s="4">
-        <v>1610612762</v>
+        <v>1610612761</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E66" s="4">
-        <v>1974</v>
+        <v>1995</v>
       </c>
       <c r="F66" s="4">
         <v>2016</v>
       </c>
       <c r="G66" s="4">
+        <v>22</v>
+      </c>
+      <c r="H66" s="4">
+        <v>1680</v>
+      </c>
+      <c r="I66" s="4">
+        <v>738</v>
+      </c>
+      <c r="J66" s="4">
+        <v>942</v>
+      </c>
+      <c r="K66" s="4">
+        <v>0.439</v>
+      </c>
+      <c r="L66" s="4">
+        <v>8</v>
+      </c>
+      <c r="M66" s="4">
+        <v>5</v>
+      </c>
+      <c r="N66" s="4">
+        <v>0</v>
+      </c>
+      <c r="O66" s="4">
+        <v>0</v>
+      </c>
+      <c r="P66" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="Q66" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" t="s">
+        <v>178</v>
+      </c>
+      <c r="B67">
+        <v>1610612761</v>
+      </c>
+      <c r="C67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D67" t="s">
+        <v>90</v>
+      </c>
+      <c r="E67">
+        <v>1995</v>
+      </c>
+      <c r="F67">
+        <v>2016</v>
+      </c>
+      <c r="G67">
+        <v>22</v>
+      </c>
+      <c r="H67">
+        <v>1680</v>
+      </c>
+      <c r="I67">
+        <v>738</v>
+      </c>
+      <c r="J67">
+        <v>942</v>
+      </c>
+      <c r="K67">
+        <v>0.439</v>
+      </c>
+      <c r="L67">
+        <v>8</v>
+      </c>
+      <c r="M67">
+        <v>5</v>
+      </c>
+      <c r="N67">
+        <v>0</v>
+      </c>
+      <c r="O67">
+        <v>0</v>
+      </c>
+      <c r="P67" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>172</v>
+      </c>
+      <c r="R67" t="s">
+        <v>180</v>
+      </c>
+      <c r="S67" t="s">
+        <v>164</v>
+      </c>
+      <c r="T67" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1610612762</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E68" s="4">
+        <v>1974</v>
+      </c>
+      <c r="F68" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G68" s="4">
         <v>43</v>
       </c>
-      <c r="H66" s="4">
+      <c r="H68" s="4">
         <v>3404</v>
       </c>
-      <c r="I66" s="4">
+      <c r="I68" s="4">
         <v>1820</v>
       </c>
-      <c r="J66" s="4">
+      <c r="J68" s="4">
         <v>1584</v>
       </c>
-      <c r="K66" s="4">
+      <c r="K68" s="4">
         <v>0.53400000000000003</v>
       </c>
-      <c r="L66" s="4">
+      <c r="L68" s="4">
         <v>25</v>
       </c>
-      <c r="M66" s="4">
+      <c r="M68" s="4">
         <v>9</v>
       </c>
-      <c r="N66" s="4">
+      <c r="N68" s="4">
         <v>2</v>
       </c>
-      <c r="O66" s="4">
-        <v>0</v>
-      </c>
-      <c r="P66" s="4" t="s">
+      <c r="O68" s="4">
+        <v>0</v>
+      </c>
+      <c r="P68" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="Q66" s="3" t="s">
+      <c r="Q68" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="R66" s="3" t="s">
+      <c r="R68" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="S66" s="3" t="s">
+      <c r="S68" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="T66" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20">
-      <c r="A67" s="3" t="s">
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B67" s="3">
+      <c r="B69" s="3">
         <v>1610612762</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D69" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E67" s="3">
+      <c r="E69" s="3">
         <v>1979</v>
       </c>
-      <c r="F67" s="3">
+      <c r="F69" s="3">
         <v>2016</v>
       </c>
-      <c r="G67" s="3">
+      <c r="G69" s="3">
         <v>38</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H69" s="3">
         <v>2994</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I69" s="3">
         <v>1659</v>
       </c>
-      <c r="J67" s="3">
+      <c r="J69" s="3">
         <v>1335</v>
       </c>
-      <c r="K67" s="3">
+      <c r="K69" s="3">
         <v>0.55400000000000005</v>
       </c>
-      <c r="L67" s="3">
+      <c r="L69" s="3">
         <v>25</v>
       </c>
-      <c r="M67" s="3">
+      <c r="M69" s="3">
         <v>9</v>
       </c>
-      <c r="N67" s="3">
+      <c r="N69" s="3">
         <v>2</v>
       </c>
-      <c r="O67" s="3">
-        <v>0</v>
-      </c>
-      <c r="P67" s="3" t="s">
+      <c r="O69" s="3">
+        <v>0</v>
+      </c>
+      <c r="P69" s="3" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20">
-      <c r="A68" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B68" s="3">
-        <v>1610612762</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E68" s="3">
-        <v>1974</v>
-      </c>
-      <c r="F68" s="3">
-        <v>1978</v>
-      </c>
-      <c r="G68" s="3">
-        <v>5</v>
-      </c>
-      <c r="H68" s="3">
-        <v>410</v>
-      </c>
-      <c r="I68" s="3">
-        <v>161</v>
-      </c>
-      <c r="J68" s="3">
-        <v>249</v>
-      </c>
-      <c r="K68" s="3">
-        <v>0.39200000000000002</v>
-      </c>
-      <c r="L68" s="3">
-        <v>0</v>
-      </c>
-      <c r="M68" s="3">
-        <v>0</v>
-      </c>
-      <c r="N68" s="3">
-        <v>0</v>
-      </c>
-      <c r="O68" s="3">
-        <v>0</v>
-      </c>
-      <c r="P68" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20">
-      <c r="A69" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B69" s="4">
-        <v>1610612764</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E69" s="4">
-        <v>1961</v>
-      </c>
-      <c r="F69" s="4">
-        <v>2016</v>
-      </c>
-      <c r="G69" s="4">
-        <v>56</v>
-      </c>
-      <c r="H69" s="4">
-        <v>4457</v>
-      </c>
-      <c r="I69" s="4">
-        <v>2005</v>
-      </c>
-      <c r="J69" s="4">
-        <v>2452</v>
-      </c>
-      <c r="K69" s="4">
-        <v>0.44900000000000001</v>
-      </c>
-      <c r="L69" s="4">
-        <v>27</v>
-      </c>
-      <c r="M69" s="4">
-        <v>7</v>
-      </c>
-      <c r="N69" s="4">
-        <v>4</v>
-      </c>
-      <c r="O69" s="4">
-        <v>1</v>
-      </c>
-      <c r="P69" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="Q69" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="R69" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="S69" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="T69" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:20">
@@ -4926,99 +4929,111 @@
         <v>178</v>
       </c>
       <c r="B70" s="3">
+        <v>1610612762</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E70" s="3">
+        <v>1974</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1978</v>
+      </c>
+      <c r="G70" s="3">
+        <v>5</v>
+      </c>
+      <c r="H70" s="3">
+        <v>410</v>
+      </c>
+      <c r="I70" s="3">
+        <v>161</v>
+      </c>
+      <c r="J70" s="3">
+        <v>249</v>
+      </c>
+      <c r="K70" s="3">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="L70" s="3">
+        <v>0</v>
+      </c>
+      <c r="M70" s="3">
+        <v>0</v>
+      </c>
+      <c r="N70" s="3">
+        <v>0</v>
+      </c>
+      <c r="O70" s="3">
+        <v>0</v>
+      </c>
+      <c r="P70" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="T70" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71" s="4">
         <v>1610612764</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="C71" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D70" s="3" t="s">
+      <c r="D71" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E70" s="3">
-        <v>1997</v>
-      </c>
-      <c r="F70" s="3">
+      <c r="E71" s="4">
+        <v>1961</v>
+      </c>
+      <c r="F71" s="4">
         <v>2016</v>
       </c>
-      <c r="G70" s="3">
-        <v>20</v>
-      </c>
-      <c r="H70" s="3">
-        <v>1516</v>
-      </c>
-      <c r="I70" s="3">
-        <v>627</v>
-      </c>
-      <c r="J70" s="3">
-        <v>889</v>
-      </c>
-      <c r="K70" s="3">
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="L70" s="3">
-        <v>6</v>
-      </c>
-      <c r="M70" s="3">
-        <v>0</v>
-      </c>
-      <c r="N70" s="3">
-        <v>0</v>
-      </c>
-      <c r="O70" s="3">
-        <v>0</v>
-      </c>
-      <c r="P70" s="6" t="s">
+      <c r="G71" s="4">
+        <v>56</v>
+      </c>
+      <c r="H71" s="4">
+        <v>4457</v>
+      </c>
+      <c r="I71" s="4">
+        <v>2005</v>
+      </c>
+      <c r="J71" s="4">
+        <v>2452</v>
+      </c>
+      <c r="K71" s="4">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="L71" s="4">
+        <v>27</v>
+      </c>
+      <c r="M71" s="4">
+        <v>7</v>
+      </c>
+      <c r="N71" s="4">
+        <v>4</v>
+      </c>
+      <c r="O71" s="4">
+        <v>1</v>
+      </c>
+      <c r="P71" s="5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="71" spans="1:20">
-      <c r="A71" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B71" s="3">
-        <v>1610612764</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E71" s="3">
-        <v>1974</v>
-      </c>
-      <c r="F71" s="3">
-        <v>1996</v>
-      </c>
-      <c r="G71" s="3">
-        <v>23</v>
-      </c>
-      <c r="H71" s="3">
-        <v>1886</v>
-      </c>
-      <c r="I71" s="3">
-        <v>887</v>
-      </c>
-      <c r="J71" s="3">
-        <v>999</v>
-      </c>
-      <c r="K71" s="3">
-        <v>0.47</v>
-      </c>
-      <c r="L71" s="3">
-        <v>13</v>
-      </c>
-      <c r="M71" s="3">
-        <v>2</v>
-      </c>
-      <c r="N71" s="3">
-        <v>3</v>
-      </c>
-      <c r="O71" s="3">
-        <v>1</v>
-      </c>
-      <c r="P71" s="6" t="s">
-        <v>148</v>
+      <c r="Q71" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="R71" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="S71" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="72" spans="1:20">
@@ -5029,37 +5044,37 @@
         <v>1610612764</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E72" s="3">
-        <v>1973</v>
+        <v>1997</v>
       </c>
       <c r="F72" s="3">
-        <v>1973</v>
+        <v>2016</v>
       </c>
       <c r="G72" s="3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="H72" s="3">
-        <v>82</v>
+        <v>1516</v>
       </c>
       <c r="I72" s="3">
-        <v>47</v>
+        <v>627</v>
       </c>
       <c r="J72" s="3">
-        <v>35</v>
+        <v>889</v>
       </c>
       <c r="K72" s="3">
-        <v>0.57299999999999995</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="L72" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="M72" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N72" s="3">
         <v>0</v>
@@ -5068,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="P72" s="6" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:20">
@@ -5079,46 +5094,46 @@
         <v>1610612764</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E73" s="3">
-        <v>1963</v>
+        <v>1974</v>
       </c>
       <c r="F73" s="3">
-        <v>1972</v>
+        <v>1996</v>
       </c>
       <c r="G73" s="3">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H73" s="3">
-        <v>813</v>
+        <v>1886</v>
       </c>
       <c r="I73" s="3">
-        <v>401</v>
+        <v>887</v>
       </c>
       <c r="J73" s="3">
-        <v>412</v>
+        <v>999</v>
       </c>
       <c r="K73" s="3">
-        <v>0.49299999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="L73" s="3">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="M73" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N73" s="3">
+        <v>3</v>
+      </c>
+      <c r="O73" s="3">
         <v>1</v>
       </c>
-      <c r="O73" s="3">
-        <v>0</v>
-      </c>
-      <c r="P73" s="3" t="s">
-        <v>155</v>
+      <c r="P73" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:20">
@@ -5129,37 +5144,37 @@
         <v>1610612764</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E74" s="3">
-        <v>1962</v>
+        <v>1973</v>
       </c>
       <c r="F74" s="3">
-        <v>1962</v>
+        <v>1973</v>
       </c>
       <c r="G74" s="3">
         <v>1</v>
       </c>
       <c r="H74" s="3">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="I74" s="3">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="J74" s="3">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="K74" s="3">
-        <v>0.312</v>
+        <v>0.57299999999999995</v>
       </c>
       <c r="L74" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M74" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N74" s="3">
         <v>0</v>
@@ -5167,8 +5182,8 @@
       <c r="O74" s="3">
         <v>0</v>
       </c>
-      <c r="P74" s="3" t="s">
-        <v>154</v>
+      <c r="P74" s="6" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="75" spans="1:20">
@@ -5179,45 +5194,145 @@
         <v>1610612764</v>
       </c>
       <c r="C75" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E75" s="3">
+        <v>1963</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1972</v>
+      </c>
+      <c r="G75" s="3">
+        <v>10</v>
+      </c>
+      <c r="H75" s="3">
+        <v>813</v>
+      </c>
+      <c r="I75" s="3">
+        <v>401</v>
+      </c>
+      <c r="J75" s="3">
+        <v>412</v>
+      </c>
+      <c r="K75" s="3">
+        <v>0.49299999999999999</v>
+      </c>
+      <c r="L75" s="3">
+        <v>7</v>
+      </c>
+      <c r="M75" s="3">
+        <v>4</v>
+      </c>
+      <c r="N75" s="3">
+        <v>1</v>
+      </c>
+      <c r="O75" s="3">
+        <v>0</v>
+      </c>
+      <c r="P75" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20">
+      <c r="A76" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="3">
+        <v>1610612764</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D75" s="3" t="s">
+      <c r="D76" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1962</v>
+      </c>
+      <c r="F76" s="3">
+        <v>1962</v>
+      </c>
+      <c r="G76" s="3">
+        <v>1</v>
+      </c>
+      <c r="H76" s="3">
+        <v>80</v>
+      </c>
+      <c r="I76" s="3">
+        <v>25</v>
+      </c>
+      <c r="J76" s="3">
+        <v>55</v>
+      </c>
+      <c r="K76" s="3">
+        <v>0.312</v>
+      </c>
+      <c r="L76" s="3">
+        <v>0</v>
+      </c>
+      <c r="M76" s="3">
+        <v>0</v>
+      </c>
+      <c r="N76" s="3">
+        <v>0</v>
+      </c>
+      <c r="O76" s="3">
+        <v>0</v>
+      </c>
+      <c r="P76" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20">
+      <c r="A77" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B77" s="3">
+        <v>1610612764</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="E75" s="3">
+      <c r="E77" s="3">
         <v>1961</v>
       </c>
-      <c r="F75" s="3">
+      <c r="F77" s="3">
         <v>1961</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G77" s="3">
         <v>1</v>
       </c>
-      <c r="H75" s="3">
+      <c r="H77" s="3">
         <v>80</v>
       </c>
-      <c r="I75" s="3">
+      <c r="I77" s="3">
         <v>18</v>
       </c>
-      <c r="J75" s="3">
+      <c r="J77" s="3">
         <v>62</v>
       </c>
-      <c r="K75" s="3">
+      <c r="K77" s="3">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L75" s="3">
-        <v>0</v>
-      </c>
-      <c r="M75" s="3">
-        <v>0</v>
-      </c>
-      <c r="N75" s="3">
-        <v>0</v>
-      </c>
-      <c r="O75" s="3">
-        <v>0</v>
-      </c>
-      <c r="P75" s="6" t="s">
+      <c r="L77" s="3">
+        <v>0</v>
+      </c>
+      <c r="M77" s="3">
+        <v>0</v>
+      </c>
+      <c r="N77" s="3">
+        <v>0</v>
+      </c>
+      <c r="O77" s="3">
+        <v>0</v>
+      </c>
+      <c r="P77" s="6" t="s">
         <v>153</v>
       </c>
     </row>

</xml_diff>